<commit_message>
cleaning up examples and adding documentation
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/template.xlsx
+++ b/examples/biochemical_models/template.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>'!!Compound'!A1</t>
   </si>
@@ -264,10 +264,10 @@
     <t>'!!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-09 23:57:33'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-09 23:57:33' objTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-10 22:57:10'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -294,48 +294,51 @@
     <t>Compound</t>
   </si>
   <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>identifiers</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>is_constant</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>ManyToOne</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>identifiers</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>is_constant</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>ManyToOne</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>column</t>
   </si>
   <si>
@@ -351,7 +354,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' id='Compound' name='Compound' description='Compound' date='2020-03-09 23:57:33' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Compound' name='Compound' description='Compound' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -366,10 +369,10 @@
     <t>!IsConstant</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-09 23:57:33' objTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' id='Reaction' name='Reaction' description='Reaction' date='2020-03-09 23:57:33' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Reaction' name='Reaction' description='Reaction' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>
@@ -926,23 +929,23 @@
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
@@ -953,7 +956,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>17</v>
@@ -972,7 +975,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
@@ -985,7 +988,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -995,24 +998,24 @@
         <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>20</v>
@@ -1023,13 +1026,13 @@
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>20</v>
@@ -1046,7 +1049,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>17</v>
@@ -1065,7 +1068,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>20</v>
@@ -1076,13 +1079,13 @@
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>22</v>
@@ -1099,7 +1102,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>24</v>
@@ -1116,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
@@ -1156,7 +1159,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1165,19 +1168,19 @@
     </row>
     <row r="2" spans="1:5" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.01" customHeight="1">
@@ -1295,7 +1298,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1310,7 +1313,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1371,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1382,25 +1385,25 @@
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.01" customHeight="1">

</xml_diff>

<commit_message>
working on documentation and converting examples to additional formats
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/template.xlsx
+++ b/examples/biochemical_models/template.xlsx
@@ -264,10 +264,10 @@
     <t>'!!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-10 22:57:10'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-12 00:22:56'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-12 00:22:56' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -354,7 +354,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' id='Compound' name='Compound' description='Compound' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Compound' name='Compound' description='Compound' date='2020-03-12 00:22:56' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -369,10 +369,10 @@
     <t>!IsConstant</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' id='Reaction' name='Reaction' description='Reaction' date='2020-03-10 22:57:10' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-12 00:22:56' objTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Reaction' name='Reaction' description='Reaction' date='2020-03-12 00:22:56' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>

</xml_diff>